<commit_message>
almost done with main.py setup
</commit_message>
<xml_diff>
--- a/experiments.xlsx
+++ b/experiments.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\topco\Dokumenti\MSc Banking and Digital Finance UCL\Modules\Dissertation\MSc_dissertation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBC4A8B6-8398-4779-AFB1-8BBB175374E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A711BCDB-77DC-4DC1-A652-C33A3E28DBD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -103,19 +103,134 @@
     <t>Exogenous variables for timeGPT??</t>
   </si>
   <si>
-    <t>for exchange rates, minutely data is only availible for the last 24 hours</t>
-  </si>
-  <si>
-    <t>For commodities minutely data is not even availible</t>
-  </si>
-  <si>
-    <t>For crypto, only last 6 hours is availible</t>
-  </si>
-  <si>
-    <t>for stocks, minutely data is availible for last 13 months</t>
-  </si>
-  <si>
-    <t>For indices, minutely data is availible only in the last 30 days</t>
+    <r>
+      <t xml:space="preserve">For </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>commodities</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> minutely data is not even availible</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">For </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>crypto</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, only last 6 hours is availible</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">for </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>stocks</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, minutely data is availible for last 13 months</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>For</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> indices</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, minutely data is availible only in the last 30 days</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">for </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>exchange rates</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, minutely data is only availible for the last 24 hours</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -600,7 +715,7 @@
   <dimension ref="D4:E24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -622,27 +737,27 @@
     </row>
     <row r="8" spans="4:5" x14ac:dyDescent="0.25">
       <c r="E8" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9" spans="4:5" x14ac:dyDescent="0.25">
       <c r="E9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="4:5" x14ac:dyDescent="0.25">
       <c r="E10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="4:5" x14ac:dyDescent="0.25">
       <c r="E11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="4:5" x14ac:dyDescent="0.25">
       <c r="E12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="16" spans="4:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
renamed exchange_rate to fx and renamed some of the results
</commit_message>
<xml_diff>
--- a/experiments.xlsx
+++ b/experiments.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\topco\Dokumenti\MSc Banking and Digital Finance UCL\Modules\Dissertation\MSc_dissertation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4D43015-3FBE-4B65-B0E9-6292D55D8FAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FE17CF1-261B-4531-B729-FED429EB48F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25800" yWindow="0" windowWidth="25800" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="21885" yWindow="2940" windowWidth="28800" windowHeight="15825" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Experiments" sheetId="1" r:id="rId1"/>
     <sheet name="notes and data restrictions" sheetId="2" r:id="rId2"/>
+    <sheet name="Experiments already ran" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="47">
   <si>
     <t>different frequency data has different seasonality and trend structures. I expect that models’ performance will change if we use different context lengths and how the performance changes depends on the frequency of data</t>
   </si>
@@ -234,6 +235,54 @@
   </si>
   <si>
     <t>(assume fixed fine-tune length)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Experiments </t>
+  </si>
+  <si>
+    <t>TOD</t>
+  </si>
+  <si>
+    <t>Index</t>
+  </si>
+  <si>
+    <t>Commodity</t>
+  </si>
+  <si>
+    <t>FX</t>
+  </si>
+  <si>
+    <t>Crypto</t>
+  </si>
+  <si>
+    <t>S&amp;P500</t>
+  </si>
+  <si>
+    <t>FTSE100</t>
+  </si>
+  <si>
+    <t>NASDAQ</t>
+  </si>
+  <si>
+    <t>DOWJ</t>
+  </si>
+  <si>
+    <t>WTI</t>
+  </si>
+  <si>
+    <t>USD/GBP</t>
+  </si>
+  <si>
+    <t>BTC</t>
+  </si>
+  <si>
+    <t>minutely</t>
+  </si>
+  <si>
+    <t>daily</t>
+  </si>
+  <si>
+    <t>weekly</t>
   </si>
 </sst>
 </file>
@@ -562,7 +611,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:D40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
@@ -722,7 +771,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5782A51B-D9F6-4A1B-8B6F-14E2E4F19BFE}">
   <dimension ref="D4:E24"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView topLeftCell="A16" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
@@ -801,4 +850,177 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CCF9C27-AE5A-4AB7-BDA6-E527BF6EC8B3}">
+  <dimension ref="A1:F35"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J25" sqref="J25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F8" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E9" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F10" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F11" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F12" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E13" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F14" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F15" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F16" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="17" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="E17" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="F18" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="19" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="F19" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="20" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="F20" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="21" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D21" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="22" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="E22" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="23" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="F23" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="24" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="F24" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="26" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D26" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="27" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="E27" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="28" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="F28" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="29" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="F29" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="30" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="F30" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="33" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D33" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="34" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="E34" t="s">
+        <v>43</v>
+      </c>
+      <c r="F34" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="35" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="F35" t="s">
+        <v>45</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>